<commit_message>
fix:SA-119,SA-120,SA-118,SA-117:Product bulk upload related and customization spelling fixed
</commit_message>
<xml_diff>
--- a/seller/app/modules/product/template/beauty_and_personal_care.xlsx
+++ b/seller/app/modules/product/template/beauty_and_personal_care.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>productCode</t>
   </si>
@@ -19,6 +19,9 @@
     <t>productName</t>
   </si>
   <si>
+    <t>basePrice</t>
+  </si>
+  <si>
     <t>MRP</t>
   </si>
   <si>
@@ -70,27 +73,24 @@
     <t>returnWindow</t>
   </si>
   <si>
-    <t>isVegetarian</t>
-  </si>
-  <si>
     <t>manufacturerName</t>
   </si>
   <si>
     <t>manufacturedDate</t>
   </si>
   <si>
-    <t>nutritionalInfo</t>
-  </si>
-  <si>
-    <t>additiveInfo</t>
-  </si>
-  <si>
-    <t>instructions</t>
+    <t>packingDate</t>
   </si>
   <si>
     <t>isCancellable</t>
   </si>
   <si>
+    <t>cancelWindow</t>
+  </si>
+  <si>
+    <t>manufacturerOrganizationName</t>
+  </si>
+  <si>
     <t>longDescription</t>
   </si>
   <si>
@@ -103,24 +103,12 @@
     <t>images</t>
   </si>
   <si>
-    <t>manufacturerOrPackerName</t>
-  </si>
-  <si>
-    <t>manufacturerOrPackerAddress</t>
-  </si>
-  <si>
     <t>commonOrGenericNameOfCommodity</t>
   </si>
   <si>
     <t>monthYearOfManufacturePackingImport</t>
   </si>
   <si>
-    <t>importerFSSAILicenseNo</t>
-  </si>
-  <si>
-    <t>brandOwnerFSSAILicenseNo</t>
-  </si>
-  <si>
     <t>data import instructions</t>
   </si>
   <si>
@@ -139,39 +127,27 @@
     <t>1234</t>
   </si>
   <si>
-    <t>Kilogram</t>
-  </si>
-  <si>
-    <t>100 kg</t>
-  </si>
-  <si>
-    <t>12 cm</t>
-  </si>
-  <si>
-    <t>1 cm</t>
+    <t>Centemeter</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>PT30M</t>
-  </si>
-  <si>
-    <t>Parle</t>
-  </si>
-  <si>
-    <t>12/1/2023</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>info</t>
+    <t>parle</t>
+  </si>
+  <si>
+    <t>2023/11/05</t>
+  </si>
+  <si>
+    <t>2023/11/06</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
+    <t>jbl</t>
+  </si>
+  <si>
     <t>long</t>
   </si>
   <si>
@@ -181,21 +157,12 @@
     <t>IRCTC</t>
   </si>
   <si>
-    <t>Pune</t>
-  </si>
-  <si>
-    <t>11/23</t>
+    <t>2023/12/07</t>
   </si>
   <si>
     <t>1. images should be a public url accessible over internet
 2. maxAllowedQty should not be 0
 3. all fields are mandatory as of now</t>
-  </si>
-  <si>
-    <t>Perfume</t>
-  </si>
-  <si>
-    <t>Fragrance</t>
   </si>
 </sst>
 </file>
@@ -220,15 +187,22 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -237,18 +211,55 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -485,6 +496,14 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="26" max="26" width="22.88"/>
+    <col customWidth="1" min="27" max="27" width="28.38"/>
+    <col customWidth="1" min="28" max="28" width="24.63"/>
+    <col customWidth="1" min="29" max="29" width="37.38"/>
+    <col customWidth="1" min="30" max="30" width="38.63"/>
+    <col customWidth="1" min="31" max="33" width="49.75"/>
+  </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -493,7 +512,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -550,19 +569,19 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
@@ -586,279 +605,136 @@
       <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+    </row>
+    <row r="2" ht="20.25" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="C2" s="6">
+        <v>400.0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>12345.0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>100.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>100.0</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="H2" s="7">
+        <v>5.0</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="J2" s="8">
+        <v>100.0</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="L2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="3">
-        <v>12345.0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="N2" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="O2" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="P2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="R2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="T2" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="U2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="V2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="3">
+      <c r="W2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y2" s="13">
         <v>1.0</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="Z2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="AA2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="AB2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="AE2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="AF2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="AG2" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI2" s="3">
-        <v>9.87654321234567E14</v>
-      </c>
-      <c r="AJ2" s="3">
-        <v>9.87654321234567E14</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="3">
-        <v>12345.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="3">
-        <v>5.0</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI3" s="3">
-        <v>9.87654321234567E14</v>
-      </c>
-      <c r="AJ3" s="3">
-        <v>9.87654321234567E14</v>
-      </c>
-      <c r="AK3" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K3">
+  <conditionalFormatting sqref="L2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E3">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(H2))&gt;0</formula>
+  <conditionalFormatting sqref="I2">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(I2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2">
       <formula1>"Fragrance,Bath Soaps and Gels,Hair Oils, Care, and Styling,Shampoos and Conditioners,Shaving and Grooming,Beard Care and Tools,Grooming Tools and Accessories,Makeup - Nail Care,Makeup - Eyes,Makeup - Face,Makeup - Lips,Makeup - Body,Makeup - Remover,Makeu"&amp;"p - Sets and Kits,Makeup - Tools and Brushes,Makeup - Kits and Combos,Skin Care - Face Cleansers,Skin Care - Hand and Feet,Body Care - Cleansers,Body Care - Moisturizers,Body Care - Loofah and Other Tools,Body Care - Bath Salt and Additives,Hair Care - Sh"&amp;"ampoo, Oils, Conditioners,Skin Care - Lotions, Moisturisers, and Creams,Skin Care - Oils and Serums,Gift Voucher"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:G3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2">
       <formula1>"0,5,12,18,28"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="R2:R3 T2:T3 Z2:Z3 AB2:AB3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="S2 W2:X2 AA2:AB2">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2">
       <formula1>"Kilogram,Grams,Meter,Centemeter"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="AD2"/>
-    <hyperlink r:id="rId2" ref="AD3"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>